<commit_message>
data collected, tiny fixes to main
</commit_message>
<xml_diff>
--- a/prototypes/post-run-analysis/EC/consolidated_relative_ec.xlsx
+++ b/prototypes/post-run-analysis/EC/consolidated_relative_ec.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3382B8DF-F75F-4637-9DFB-75C627624885}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68295F4-C5FC-47AE-B32E-D8E2FD96F783}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,8 +447,8 @@
   <dimension ref="A1:T91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L90" sqref="L90"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P88" sqref="P88:P91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,6 +1598,20 @@
       <c r="L41">
         <v>21</v>
       </c>
+      <c r="M41">
+        <v>22</v>
+      </c>
+      <c r="N41">
+        <f t="shared" ref="N41:N87" si="11">AVERAGE(B41:M41)</f>
+        <v>15.333333333333334</v>
+      </c>
+      <c r="O41">
+        <v>15</v>
+      </c>
+      <c r="P41">
+        <f>O41*100/31</f>
+        <v>48.387096774193552</v>
+      </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1635,6 +1649,20 @@
       </c>
       <c r="L42">
         <v>2</v>
+      </c>
+      <c r="M42">
+        <v>2</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="11"/>
+        <v>6.75</v>
+      </c>
+      <c r="O42">
+        <v>7</v>
+      </c>
+      <c r="P42">
+        <f t="shared" ref="P42:P44" si="12">O42*100/31</f>
+        <v>22.580645161290324</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -1647,7 +1675,45 @@
       <c r="C43">
         <v>0</v>
       </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
       <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -1659,9 +1725,61 @@
         <f>31-B43-B42-B41</f>
         <v>16</v>
       </c>
+      <c r="C44">
+        <f t="shared" ref="C44:M44" si="13">31-C43-C42-C41</f>
+        <v>7</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
       <c r="F44">
-        <f>31-F43-F42-F41</f>
+        <f t="shared" si="13"/>
         <v>9</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="N44">
+        <f t="shared" ref="N44" si="14">31-N43-N42-N41</f>
+        <v>8.9166666666666661</v>
+      </c>
+      <c r="O44">
+        <f t="shared" ref="O44" si="15">31-O43-O42-O41</f>
+        <v>9</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="12"/>
+        <v>29.032258064516128</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -1669,7 +1787,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -1706,8 +1824,22 @@
       <c r="L49">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <v>7</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="11"/>
+        <v>6.25</v>
+      </c>
+      <c r="O49">
+        <v>6</v>
+      </c>
+      <c r="P49">
+        <f>O49*100/26</f>
+        <v>23.076923076923077</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -1744,8 +1876,22 @@
       <c r="L50">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50">
+        <v>3</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="11"/>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="O50">
+        <v>5</v>
+      </c>
+      <c r="P50">
+        <f t="shared" ref="P50:P52" si="16">O50*100/26</f>
+        <v>19.23076923076923</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -1758,20 +1904,46 @@
       <c r="D51">
         <v>1</v>
       </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
       <c r="F51">
         <v>0</v>
       </c>
       <c r="G51">
         <v>1</v>
       </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
       <c r="I51">
         <v>1</v>
       </c>
       <c r="J51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="11"/>
+        <v>0.5</v>
+      </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="16"/>
+        <v>3.8461538461538463</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -1779,17 +1951,69 @@
         <f>26-B51-B50-B49</f>
         <v>17</v>
       </c>
+      <c r="C52">
+        <f t="shared" ref="C52:M52" si="17">26-C51-C50-C49</f>
+        <v>10</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="17"/>
+        <v>18</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="17"/>
+        <v>15</v>
+      </c>
       <c r="F52">
-        <f>26-F51-F50-F49</f>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <f t="shared" si="17"/>
+        <v>15</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="17"/>
+        <v>16</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="17"/>
+        <v>14</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="17"/>
+        <v>17</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="17"/>
+        <v>11</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="17"/>
+        <v>15</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="17"/>
+        <v>16</v>
+      </c>
+      <c r="N52">
+        <f t="shared" ref="N52" si="18">26-N51-N50-N49</f>
+        <v>14.583333333333332</v>
+      </c>
+      <c r="O52">
+        <f t="shared" ref="O52" si="19">26-O51-O50-O49</f>
+        <v>14</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="16"/>
+        <v>53.846153846153847</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -1826,8 +2050,22 @@
       <c r="L57">
         <v>7</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57">
+        <v>4</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="11"/>
+        <v>3.9166666666666665</v>
+      </c>
+      <c r="O57">
+        <v>4</v>
+      </c>
+      <c r="P57">
+        <f>O57*100/17</f>
+        <v>23.529411764705884</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -1864,8 +2102,22 @@
       <c r="L58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="O58">
+        <v>2</v>
+      </c>
+      <c r="P58">
+        <f t="shared" ref="P58:P60" si="20">O58*100/17</f>
+        <v>11.764705882352942</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1893,11 +2145,31 @@
       <c r="I59">
         <v>2</v>
       </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
       <c r="K59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>2</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="11"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="O59">
+        <v>1</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="20"/>
+        <v>5.882352941176471</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>18</v>
       </c>
@@ -1905,17 +2177,69 @@
         <f>17-B59-B58-B57</f>
         <v>12</v>
       </c>
+      <c r="C60">
+        <f t="shared" ref="C60:M60" si="21">17-C59-C58-C57</f>
+        <v>8</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="21"/>
+        <v>11</v>
+      </c>
       <c r="F60">
-        <f>17-F59-F58-F57</f>
+        <f t="shared" si="21"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <f t="shared" si="21"/>
+        <v>11</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="21"/>
+        <v>10</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="21"/>
+        <v>10</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="M60">
+        <f t="shared" si="21"/>
+        <v>10</v>
+      </c>
+      <c r="N60">
+        <f t="shared" ref="N60" si="22">17-N59-N58-N57</f>
+        <v>9.9166666666666679</v>
+      </c>
+      <c r="O60">
+        <f t="shared" ref="O60" si="23">17-O59-O58-O57</f>
+        <v>10</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="20"/>
+        <v>58.823529411764703</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -1952,8 +2276,22 @@
       <c r="L64">
         <v>10</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M64">
+        <v>9</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="11"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="O64">
+        <v>6</v>
+      </c>
+      <c r="P64">
+        <f>O64*100/24</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -1990,8 +2328,22 @@
       <c r="L65">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M65">
+        <v>6</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="O65">
+        <v>6</v>
+      </c>
+      <c r="P65">
+        <f t="shared" ref="P65:P67" si="24">O65*100/24</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -2004,17 +2356,46 @@
       <c r="D66">
         <v>1</v>
       </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
       <c r="F66">
         <v>1</v>
       </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
       <c r="H66">
         <v>1</v>
       </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
       <c r="J66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>1</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="11"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>18</v>
       </c>
@@ -2022,17 +2403,69 @@
         <f>24-B66-B65-B64</f>
         <v>14</v>
       </c>
+      <c r="C67">
+        <f t="shared" ref="C67:M67" si="25">24-C66-C65-C64</f>
+        <v>9</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="25"/>
+        <v>13</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="25"/>
+        <v>15</v>
+      </c>
       <c r="F67">
-        <f>24-F66-F65-F64</f>
+        <f t="shared" si="25"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <f t="shared" si="25"/>
+        <v>13</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="25"/>
+        <v>9</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="25"/>
+        <v>15</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="25"/>
+        <v>12</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="25"/>
+        <v>8</v>
+      </c>
+      <c r="M67">
+        <f t="shared" si="25"/>
+        <v>8</v>
+      </c>
+      <c r="N67">
+        <f t="shared" ref="N67" si="26">24-N66-N65-N64</f>
+        <v>11.25</v>
+      </c>
+      <c r="O67">
+        <f t="shared" ref="O67" si="27">24-O66-O65-O64</f>
+        <v>12</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="24"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -2069,8 +2502,22 @@
       <c r="L72">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M72">
+        <v>4</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="11"/>
+        <v>2.8333333333333335</v>
+      </c>
+      <c r="O72">
+        <v>3</v>
+      </c>
+      <c r="P72">
+        <f>O72*100/11</f>
+        <v>27.272727272727273</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -2107,8 +2554,22 @@
       <c r="L73">
         <v>3</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M73">
+        <v>2</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="11"/>
+        <v>3.4166666666666665</v>
+      </c>
+      <c r="O73">
+        <v>3</v>
+      </c>
+      <c r="P73">
+        <f t="shared" ref="P73:P75" si="28">O73*100/11</f>
+        <v>27.272727272727273</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -2118,17 +2579,49 @@
       <c r="C74">
         <v>0</v>
       </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
       <c r="G74">
         <v>1</v>
       </c>
       <c r="H74">
         <v>1</v>
       </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
       <c r="J74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>1</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="11"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
+      </c>
+      <c r="P74">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>18</v>
       </c>
@@ -2136,13 +2629,69 @@
         <f>11-B74-B73-B72</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <f t="shared" ref="C75:M75" si="29">11-C74-C73-C72</f>
+        <v>4</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="29"/>
+        <v>6</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="29"/>
+        <v>6</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="M75">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="N75">
+        <f t="shared" ref="N75" si="30">11-N74-N73-N72</f>
+        <v>4.4166666666666661</v>
+      </c>
+      <c r="O75">
+        <f t="shared" ref="O75" si="31">11-O74-O73-O72</f>
+        <v>5</v>
+      </c>
+      <c r="P75">
+        <f t="shared" si="28"/>
+        <v>45.454545454545453</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -2179,8 +2728,22 @@
       <c r="L80">
         <v>10</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M80">
+        <v>9</v>
+      </c>
+      <c r="N80">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="O80">
+        <v>7</v>
+      </c>
+      <c r="P80">
+        <f>O80*100/19</f>
+        <v>36.842105263157897</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>2</v>
       </c>
@@ -2217,8 +2780,22 @@
       <c r="L81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M81">
+        <v>3</v>
+      </c>
+      <c r="N81">
+        <f t="shared" si="11"/>
+        <v>3.25</v>
+      </c>
+      <c r="O81">
+        <v>3</v>
+      </c>
+      <c r="P81">
+        <f t="shared" ref="P81:P83" si="32">O81*100/19</f>
+        <v>15.789473684210526</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>3</v>
       </c>
@@ -2228,20 +2805,49 @@
       <c r="C82">
         <v>0</v>
       </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
       <c r="F82">
         <v>1</v>
       </c>
       <c r="G82">
         <v>1</v>
       </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
       <c r="J82">
         <v>1</v>
       </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
       <c r="L82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <f t="shared" si="11"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O82">
+        <v>0</v>
+      </c>
+      <c r="P82">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>18</v>
       </c>
@@ -2249,13 +2855,69 @@
         <f>19-B82-B81-B80</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <f t="shared" ref="C83:M83" si="33">19-C82-C81-C80</f>
+        <v>7</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="33"/>
+        <v>10</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="33"/>
+        <v>9</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="33"/>
+        <v>8</v>
+      </c>
+      <c r="G83">
+        <f t="shared" si="33"/>
+        <v>7</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="33"/>
+        <v>7</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="33"/>
+        <v>11</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="33"/>
+        <v>7</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="33"/>
+        <v>10</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="33"/>
+        <v>7</v>
+      </c>
+      <c r="M83">
+        <f t="shared" si="33"/>
+        <v>7</v>
+      </c>
+      <c r="N83">
+        <f t="shared" ref="N83" si="34">19-N82-N81-N80</f>
+        <v>8.4166666666666679</v>
+      </c>
+      <c r="O83">
+        <f t="shared" ref="O83" si="35">19-O82-O81-O80</f>
+        <v>9</v>
+      </c>
+      <c r="P83">
+        <f t="shared" si="32"/>
+        <v>47.368421052631582</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -2292,8 +2954,22 @@
       <c r="L88">
         <v>13</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M88">
+        <v>8</v>
+      </c>
+      <c r="N88">
+        <f>AVERAGE(B88:M88)</f>
+        <v>7.916666666666667</v>
+      </c>
+      <c r="O88">
+        <v>8</v>
+      </c>
+      <c r="P88">
+        <f>O88*100/67</f>
+        <v>11.940298507462687</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>2</v>
       </c>
@@ -2330,8 +3006,22 @@
       <c r="L89">
         <v>7</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M89">
+        <v>16</v>
+      </c>
+      <c r="N89">
+        <f t="shared" ref="N89:N91" si="36">AVERAGE(B89:M89)</f>
+        <v>11.583333333333334</v>
+      </c>
+      <c r="O89">
+        <v>12</v>
+      </c>
+      <c r="P89">
+        <f t="shared" ref="P89:P91" si="37">O89*100/67</f>
+        <v>17.910447761194028</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>3</v>
       </c>
@@ -2347,9 +3037,15 @@
       <c r="E90">
         <v>1</v>
       </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
       <c r="G90">
         <v>1</v>
       </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
       <c r="I90">
         <v>1</v>
       </c>
@@ -2359,14 +3055,87 @@
       <c r="K90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <v>0</v>
+      </c>
+      <c r="N90">
+        <f t="shared" si="36"/>
+        <v>0.75</v>
+      </c>
+      <c r="O90">
+        <v>1</v>
+      </c>
+      <c r="P90">
+        <f t="shared" si="37"/>
+        <v>1.4925373134328359</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>18</v>
       </c>
       <c r="B91">
         <f>67-B90-B89-B88</f>
         <v>52</v>
+      </c>
+      <c r="C91">
+        <f t="shared" ref="C91:M91" si="38">67-C90-C89-C88</f>
+        <v>36</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="38"/>
+        <v>56</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="38"/>
+        <v>48</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="38"/>
+        <v>42</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="38"/>
+        <v>48</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="38"/>
+        <v>43</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="38"/>
+        <v>53</v>
+      </c>
+      <c r="J91">
+        <f t="shared" si="38"/>
+        <v>48</v>
+      </c>
+      <c r="K91">
+        <f t="shared" si="38"/>
+        <v>45</v>
+      </c>
+      <c r="L91">
+        <f t="shared" si="38"/>
+        <v>47</v>
+      </c>
+      <c r="M91">
+        <f t="shared" si="38"/>
+        <v>43</v>
+      </c>
+      <c r="N91">
+        <f t="shared" ref="N91" si="39">67-N90-N89-N88</f>
+        <v>46.75</v>
+      </c>
+      <c r="O91">
+        <f t="shared" ref="O91" si="40">67-O90-O89-O88</f>
+        <v>46</v>
+      </c>
+      <c r="P91">
+        <f t="shared" si="37"/>
+        <v>68.656716417910445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>